<commit_message>
Completed 4 Arrays problem
</commit_message>
<xml_diff>
--- a/Love Babber Roadmap/FINAL450.xlsx
+++ b/Love Babber Roadmap/FINAL450.xlsx
@@ -458,7 +458,7 @@
         <v xml:space="preserve">Move all the negative elements to one side of the array </v>
       </c>
       <c r="C10" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="11">
@@ -469,7 +469,7 @@
         <v>Find the Union and Intersection of the two sorted arrays.</v>
       </c>
       <c r="C11" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="12">
@@ -480,7 +480,7 @@
         <v>Write a program to cyclically rotate an array by one.</v>
       </c>
       <c r="C12" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="13">
@@ -491,7 +491,7 @@
         <v>find Largest sum contiguous Subarray [V. IMP]</v>
       </c>
       <c r="C13" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
2 More Array Problems
</commit_message>
<xml_diff>
--- a/Love Babber Roadmap/FINAL450.xlsx
+++ b/Love Babber Roadmap/FINAL450.xlsx
@@ -513,7 +513,7 @@
         <v>Minimum no. of Jumps to reach end of an array</v>
       </c>
       <c r="C15" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="16">
@@ -524,7 +524,7 @@
         <v>find duplicate in an array of N+1 Integers</v>
       </c>
       <c r="C16" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="17">

</xml_diff>

<commit_message>
added 1 problem to sheet
</commit_message>
<xml_diff>
--- a/Love Babber Roadmap/FINAL450.xlsx
+++ b/Love Babber Roadmap/FINAL450.xlsx
@@ -803,6 +803,12 @@
       </c>
     </row>
     <row r="42">
+      <c r="A42" t="str">
+        <v>Array</v>
+      </c>
+      <c r="B42" t="str">
+        <v>House Robber Problem</v>
+      </c>
       <c r="C42" t="str">
         <v>&lt;-&gt;</v>
       </c>

</xml_diff>

<commit_message>
Skillrack DC and Arrays Problems
</commit_message>
<xml_diff>
--- a/Love Babber Roadmap/FINAL450.xlsx
+++ b/Love Babber Roadmap/FINAL450.xlsx
@@ -590,7 +590,7 @@
         <v>Best time to buy and Sell stock</v>
       </c>
       <c r="C22" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="23">
@@ -810,7 +810,7 @@
         <v>House Robber Problem</v>
       </c>
       <c r="C42" t="str">
-        <v>&lt;-&gt;</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="43">

</xml_diff>